<commit_message>
menambahkan field makul 6 di dosen lb admin
</commit_message>
<xml_diff>
--- a/public/contoh-excel/dosenlb.xlsx
+++ b/public/contoh-excel/dosenlb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14025" windowHeight="12150"/>
+    <workbookView windowWidth="28170" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>email</t>
   </si>
@@ -112,6 +112,21 @@
     <t>honor_mk_5</t>
   </si>
   <si>
+    <t>matkul_6</t>
+  </si>
+  <si>
+    <t>nominal_matkul_6</t>
+  </si>
+  <si>
+    <t>sks_matkul_6</t>
+  </si>
+  <si>
+    <t>jml_hadir_mkl_6</t>
+  </si>
+  <si>
+    <t>honor_mk_6</t>
+  </si>
+  <si>
     <t>anggota_klp_dosen</t>
   </si>
   <si>
@@ -133,7 +148,7 @@
     <t>honor_yang_dibayar</t>
   </si>
   <si>
-    <t>tia@gmail.com</t>
+    <t xml:space="preserve">putranugraha@primakara.ac.id </t>
   </si>
   <si>
     <t>Tia</t>
@@ -151,13 +166,16 @@
     <t>Bahasa Arab</t>
   </si>
   <si>
-    <t>Bahasa Kawi</t>
+    <t>Bahasa Indonesia</t>
   </si>
   <si>
     <t xml:space="preserve">Bahasa Prancis </t>
   </si>
   <si>
-    <t xml:space="preserve">Bahasa Jawa </t>
+    <t>Bahasa Thailand</t>
+  </si>
+  <si>
+    <t>Bahasa Inggris</t>
   </si>
 </sst>
 </file>
@@ -166,9 +184,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -194,11 +212,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,8 +227,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,6 +250,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -240,6 +289,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -248,31 +304,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,38 +334,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,187 +350,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,39 +541,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -576,11 +561,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,6 +609,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -628,142 +646,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1099,15 +1117,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.8" customWidth="true"/>
+    <col min="1" max="1" width="18.1" customWidth="true"/>
     <col min="5" max="5" width="17.5" customWidth="true"/>
     <col min="6" max="6" width="17" customWidth="true"/>
     <col min="7" max="7" width="12.2" customWidth="true"/>
@@ -1136,16 +1154,21 @@
     <col min="30" max="30" width="11.6" customWidth="true"/>
     <col min="31" max="31" width="13.8" customWidth="true"/>
     <col min="32" max="32" width="10.6" customWidth="true"/>
-    <col min="33" max="33" width="15.9" customWidth="true"/>
-    <col min="34" max="34" width="13.9" customWidth="true"/>
+    <col min="33" max="33" width="11.4" customWidth="true"/>
+    <col min="34" max="34" width="16.2" customWidth="true"/>
     <col min="35" max="35" width="11.6" customWidth="true"/>
-    <col min="36" max="36" width="12.5" customWidth="true"/>
-    <col min="37" max="37" width="9.3"/>
-    <col min="38" max="38" width="10.7" customWidth="true"/>
-    <col min="39" max="39" width="17.7" customWidth="true"/>
+    <col min="36" max="36" width="13.8" customWidth="true"/>
+    <col min="37" max="37" width="10.6" customWidth="true"/>
+    <col min="38" max="38" width="15.9" customWidth="true"/>
+    <col min="39" max="39" width="13.9" customWidth="true"/>
+    <col min="40" max="40" width="11.6" customWidth="true"/>
+    <col min="41" max="41" width="12.5" customWidth="true"/>
+    <col min="42" max="42" width="9.3"/>
+    <col min="43" max="43" width="10.7" customWidth="true"/>
+    <col min="44" max="44" width="17.7" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:44">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1263,31 +1286,46 @@
       <c r="AM1" t="s">
         <v>38</v>
       </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:44">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>2024</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G2">
         <v>50000</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I2">
         <v>50000</v>
@@ -1302,7 +1340,7 @@
         <v>5000</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="N2">
         <v>50000</v>
@@ -1317,7 +1355,7 @@
         <v>2000</v>
       </c>
       <c r="R2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="S2">
         <v>2000</v>
@@ -1332,7 +1370,7 @@
         <v>3000</v>
       </c>
       <c r="W2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="X2">
         <v>50000</v>
@@ -1347,7 +1385,7 @@
         <v>5000</v>
       </c>
       <c r="AB2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="AC2">
         <v>50000</v>
@@ -1361,31 +1399,46 @@
       <c r="AF2">
         <v>5000</v>
       </c>
-      <c r="AG2">
-        <v>0</v>
+      <c r="AG2" t="s">
+        <v>53</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AK2">
-        <v>12000000</v>
+        <v>5000</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>12000000</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
         <v>12000000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="tia@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="putranugraha@primakara.ac.id " tooltip="mailto:putranugraha@primakara.ac.id "/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>